<commit_message>
2nd commit by Dev-B
</commit_message>
<xml_diff>
--- a/Sush 23dec23.xlsx
+++ b/Sush 23dec23.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
   <si>
     <t>https://drive.google.com/file/d/10cN0y84dJk-Ci7uI8FylLhzwZSqBvHhY/view?usp=drive_link</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Creat Github Acc And Create Reposi</t>
   </si>
   <si>
-    <t>Creat Github Acc And Create Reposi ,Version control</t>
-  </si>
-  <si>
     <t>https://drive.google.com/file/d/1WjdgOayM8iK_7ScE5dgpOMkPeqA2VCLb/view?usp=drive_link</t>
   </si>
   <si>
@@ -78,9 +75,6 @@
     <t>No Class</t>
   </si>
   <si>
-    <t>Realese Branch</t>
-  </si>
-  <si>
     <t>https://drive.google.com/file/d/1-3dlZBw7j-BflZVu0XBlVhFcjAyz6OMG/view?usp=drive_link</t>
   </si>
   <si>
@@ -145,22 +139,44 @@
   </si>
   <si>
     <t xml:space="preserve">How trigger Task on jenkins </t>
+  </si>
+  <si>
+    <t>Backup &amp;Restore on Jenkins</t>
+  </si>
+  <si>
+    <t>How To get backup and restore on jenkins</t>
+  </si>
+  <si>
+    <t>what is branch AndRealese Branch</t>
+  </si>
+  <si>
+    <t>Release Branch,Customer Branch release /SIT branch and UAT branch creat on git command,haow to ad tag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creat Github Acc And Create Reposi ,Version control,How can we use git </t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1ERVq2oBN4DI3Q_J06SuwfuQ0CmrttcgW/view?usp=drive_link</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1wQEWfgqBOgitgPtuMjo_NOqdVyJexh_g/view?usp=drive_link</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1jcaeyXZ7wB5FszOyHUBDcd6gsvIVXVw8/view?usp=drive_link</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1sBxaxuCPIHtgcBWztCTZRqotSnQAYIaC/view?usp=drive_link</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/13l_p2dR6IiVBZwlgiwm0893qCnO8uL58/view?usp=drive_link</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -193,21 +209,21 @@
     </font>
     <font>
       <b/>
-      <sz val="20"/>
+      <u/>
+      <sz val="14"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="20"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <u/>
       <sz val="14"/>
       <color theme="10"/>
@@ -250,26 +266,24 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="15" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -572,342 +586,378 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="3" width="91.42578125" customWidth="1"/>
-    <col min="4" max="4" width="118.42578125" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16" style="5" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="91.42578125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="122.85546875" style="5" customWidth="1"/>
+    <col min="5" max="6" width="9.140625" style="5"/>
+    <col min="7" max="7" width="19.42578125" style="5" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-    </row>
-    <row r="2" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+    <row r="1" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+    </row>
+    <row r="2" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-    </row>
-    <row r="3" spans="1:4" s="6" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="5" t="s">
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+    </row>
+    <row r="3" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="6" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-    </row>
-    <row r="5" spans="1:4" s="6" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="1:4" s="6" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-    </row>
-    <row r="7" spans="1:4" s="6" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="1:4" s="6" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="1:4" s="9" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="7">
+        <v>45274</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+    </row>
+    <row r="5" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="7">
+        <v>45275</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+    </row>
+    <row r="6" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="7">
+        <v>45276</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+    </row>
+    <row r="7" spans="1:4" s="4" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="7">
+        <v>45278</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="4" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="7">
+        <v>45279</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="4" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="7">
-        <v>45278</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="9" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>45280</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="4" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="7">
-        <v>45279</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="9" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>45281</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="4" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="7">
-        <v>45280</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="9" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>45282</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="8"/>
+    </row>
+    <row r="12" spans="1:4" s="4" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="7">
-        <v>45281</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="10" t="s">
+        <v>45283</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="4" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="7">
+        <v>45284</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="8"/>
+    </row>
+    <row r="14" spans="1:4" s="4" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="7">
+        <v>45285</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="8"/>
+    </row>
+    <row r="15" spans="1:4" s="4" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="7">
+        <v>45286</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="4" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="7">
+        <v>45287</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="4" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="7">
+        <v>45288</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="4" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="7">
+        <v>45289</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" s="9" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="7">
-        <v>45282</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="10"/>
-    </row>
-    <row r="14" spans="1:4" s="9" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="7">
-        <v>45283</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="10" t="s">
+      <c r="C18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="4" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="7">
+        <v>45290</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="6"/>
+    </row>
+    <row r="20" spans="1:4" s="4" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="7">
+        <v>45291</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="4" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="10">
+        <v>45292</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="6"/>
+    </row>
+    <row r="22" spans="1:4" s="4" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="7">
+        <v>45293</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="4" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="7">
+        <v>45294</v>
+      </c>
+      <c r="B23" s="6"/>
+      <c r="C23" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="6"/>
+    </row>
+    <row r="24" spans="1:4" s="4" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="7">
+        <v>45295</v>
+      </c>
+      <c r="B24" s="6"/>
+      <c r="C24" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="6"/>
+    </row>
+    <row r="25" spans="1:4" s="4" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="7">
+        <v>45296</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" s="6"/>
+    </row>
+    <row r="26" spans="1:4" s="4" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="10">
+        <v>45297</v>
+      </c>
+      <c r="B26" s="6"/>
+      <c r="C26" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="6"/>
+    </row>
+    <row r="27" spans="1:4" s="4" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="7">
+        <v>45298</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" s="4" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+    </row>
+    <row r="29" spans="1:4" s="4" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="9" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="7">
-        <v>45284</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="10"/>
-    </row>
-    <row r="16" spans="1:4" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="7">
-        <v>45285</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="10"/>
-    </row>
-    <row r="17" spans="1:4" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="7">
-        <v>45286</v>
-      </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" s="10"/>
-    </row>
-    <row r="18" spans="1:4" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="7">
-        <v>45287</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="7">
-        <v>45288</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" s="9" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="7">
-        <v>45289</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" s="9" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="7">
-        <v>45290</v>
-      </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-    </row>
-    <row r="22" spans="1:4" s="9" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="7">
-        <v>45291</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" s="9" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="12">
-        <v>45292</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-    </row>
-    <row r="24" spans="1:4" s="9" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="7">
-        <v>45293</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" s="9" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="7">
-        <v>45294</v>
-      </c>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-    </row>
-    <row r="26" spans="1:4" s="9" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D26" s="4"/>
-    </row>
-    <row r="27" spans="1:4" s="9" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-    </row>
-    <row r="28" spans="1:4" s="9" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" s="9" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-    </row>
-    <row r="30" spans="1:4" s="9" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-    </row>
-    <row r="31" spans="1:4" s="9" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-    </row>
-    <row r="32" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-    </row>
-    <row r="34" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
+    <row r="30" spans="1:4" s="4" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+    </row>
+    <row r="31" spans="1:4" s="4" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+    </row>
+    <row r="32" spans="1:4" s="4" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+    </row>
+    <row r="33" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="9"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+    </row>
+    <row r="34" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="9"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+    </row>
+    <row r="35" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="9"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -915,13 +965,17 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C9" r:id="rId1"/>
-    <hyperlink ref="C11" r:id="rId2"/>
+    <hyperlink ref="C18" r:id="rId2"/>
     <hyperlink ref="C20" r:id="rId3"/>
     <hyperlink ref="C22" r:id="rId4"/>
-    <hyperlink ref="C24" r:id="rId5"/>
+    <hyperlink ref="C27" r:id="rId5"/>
+    <hyperlink ref="C26" r:id="rId6"/>
+    <hyperlink ref="C25" r:id="rId7"/>
+    <hyperlink ref="C24" r:id="rId8"/>
+    <hyperlink ref="C7" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
 
@@ -940,36 +994,36 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="B3" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
+      <c r="B3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
       <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
+        <v>45286</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <v>45287</v>
+      </c>
+      <c r="C6" t="s">
         <v>26</v>
-      </c>
-      <c r="D4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="3">
-        <v>45286</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="3">
-        <v>45287</v>
-      </c>
-      <c r="C6" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>